<commit_message>
checked that backup xlsx not tracked
</commit_message>
<xml_diff>
--- a/inst/extdata/z-shift-helper.xlsx
+++ b/inst/extdata/z-shift-helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrminter\Documents\git\rpemepma\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E4CA20-D0C0-4586-A722-D79D5C0571BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74677B9-873C-4586-B142-8D4372C1A671}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="8115" xr2:uid="{5F385284-567F-48F5-9CD0-308CBCB548D2}"/>
   </bookViews>
@@ -390,7 +390,7 @@
   <dimension ref="B2:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>